<commit_message>
Forgot to add phone number to Aarhus Havn (otherwise no contact channels are displayed)
</commit_message>
<xml_diff>
--- a/sandbox/AAK/AARHUS_minified.xlsx
+++ b/sandbox/AAK/AARHUS_minified.xlsx
@@ -358,18 +358,18 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.7813765182186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.2388663967611"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.5627530364373"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.6356275303644"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="34.5991902834008"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="44.2388663967611"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="35.6720647773279"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="34.8137651821862"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="44.5627530364373"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="35.9919028340081"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.0688259109312"/>
     <col collapsed="false" hidden="false" max="13" min="12" style="0" width="11.7813765182186"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="26" min="15" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.67611336032389"/>
   </cols>
@@ -479,10 +479,10 @@
   </sheetPr>
   <dimension ref="A1:P65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -491,17 +491,17 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.60728744939271"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.78542510121457"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="2.1417004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0323886639676"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="34.5991902834008"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="40.5991902834008"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="36.4210526315789"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="2.03643724696356"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="34.8137651821862"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="40.919028340081"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="36.7408906882591"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.92712550607287"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="38.3481781376518"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.3522267206478"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="36.4210526315789"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="38.668016194332"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="36.7408906882591"/>
     <col collapsed="false" hidden="false" max="24" min="16" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="8.67611336032389"/>
   </cols>
@@ -581,6 +581,9 @@
       <c r="K2" s="0" t="s">
         <v>38</v>
       </c>
+      <c r="L2" s="0" t="n">
+        <v>12345678</v>
+      </c>
       <c r="M2" s="0" t="s">
         <v>39</v>
       </c>
@@ -618,6 +621,9 @@
       </c>
       <c r="K3" s="0" t="s">
         <v>38</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>87654321</v>
       </c>
       <c r="M3" s="0" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
Added an extra enhedstype to the AARHUS_minified spreadsheet
</commit_message>
<xml_diff>
--- a/sandbox/AAK/AARHUS_minified.xlsx
+++ b/sandbox/AAK/AARHUS_minified.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t xml:space="preserve">operation</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t xml:space="preserve">ÅRHUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0034fa1f-b1ef-4764-8505-c5b9ca43aaa9</t>
   </si>
   <si>
     <t xml:space="preserve">Rådhuset</t>
@@ -358,18 +361,18 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.7813765182186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.5627530364373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.8825910931174"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8502024291498"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="34.8137651821862"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="44.5627530364373"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="35.9919028340081"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.0283400809717"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="44.8825910931174"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="36.3117408906883"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.1740890688259"/>
     <col collapsed="false" hidden="false" max="13" min="12" style="0" width="11.7813765182186"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="26" min="15" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.67611336032389"/>
   </cols>
@@ -479,10 +482,10 @@
   </sheetPr>
   <dimension ref="A1:P65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -491,17 +494,17 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.60728744939271"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.78542510121457"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="2.03643724696356"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="34.8137651821862"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="40.919028340081"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="36.7408906882591"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="1.92712550607287"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.0283400809717"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="41.2388663967611"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="37.0647773279352"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.92712550607287"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="38.668016194332"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="36.7408906882591"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="38.9919028340081"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="37.0647773279352"/>
     <col collapsed="false" hidden="false" max="24" min="16" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="8.67611336032389"/>
   </cols>
@@ -611,10 +614,10 @@
         <v>17</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>8000</v>
@@ -626,7 +629,7 @@
         <v>87654321</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O3" s="0" t="s">
         <v>14</v>

</xml_diff>